<commit_message>
changed training metric and LR gridsearch
</commit_message>
<xml_diff>
--- a/output/train_experiments_results - challenge2.xlsx
+++ b/output/train_experiments_results - challenge2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\master\udg\CAD\project\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C52BDE-3C79-4487-8439-D10A73DBE6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30485FE6-C1B7-4D2F-835D-57C087ABBB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Experiment Count</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>but I think it didn't converge</t>
+  </si>
+  <si>
+    <t>Scoring metric</t>
+  </si>
+  <si>
+    <t>accuracy'</t>
+  </si>
+  <si>
+    <t>'accuracy'</t>
+  </si>
+  <si>
+    <t>f1_weighted'</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'penalty': 'l1', 'solver': 'liblinear'}</t>
   </si>
 </sst>
 </file>
@@ -188,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -260,11 +275,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,11 +320,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="41">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -700,53 +749,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="B2:I6" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}" name="Table2" displayName="Table2" ref="B13:AB19" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="B13:AB19" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}"/>
-  <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{B1948067-CB65-4206-AE71-0D57640D7089}" name="Experiment Count" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{FDDCB198-EAE1-4ED4-A066-F8DBAC98C717}" name="Features" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{83D1AD7E-916A-4241-B599-9349DCDB2027}" name="N_Features" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{70DAF01F-DAE6-4B77-9BDB-7F5053A6F854}" name="Data Shuffled" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{3B5E59E9-2BF5-4D6D-816E-23251AFDB13E}" name="Feature Selection" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{F7473F45-1D6D-409F-9883-1FD36FD545E3}" name="Model" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{90C55BBC-BCBC-4A00-8864-5A767EA01E45}" name="Multiclass handling" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{75867AB3-1849-4FCA-B58F-BE8AEF3B207D}" name="Imbalance handling" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{B2F22562-6078-45C9-A5D5-49F1FBF2A4F1}" name="Accuracy" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{72664E3E-D59C-4D9C-8541-496AB288C8B6}" name="Balanced accuracy" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{0FEE43E7-8EFC-4D86-86B0-C5FE824F8CBB}" name="Weighted f1" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{957B2BF0-94D0-4D47-92EE-5F281E10A28D}" name="BCC Specificity" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{BC24D8AD-88D3-42DE-B472-81BDDB9C87B9}" name="BCC sensitivity" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{69470701-5DB0-4C11-AF39-0426EC578174}" name="BCC precision" dataDxfId="13"/>
-    <tableColumn id="26" xr3:uid="{45ED09DC-26C9-4D46-8786-471740B03DA6}" name="BCC F1 score" dataDxfId="12"/>
-    <tableColumn id="27" xr3:uid="{728ACE6E-7304-449C-A3BC-0DFA6F380155}" name="BCC AUC " dataDxfId="11"/>
-    <tableColumn id="18" xr3:uid="{99DAD431-5D89-4923-BC81-A35FE3C6B664}" name="MEL Specificity" dataDxfId="10"/>
-    <tableColumn id="19" xr3:uid="{AD2D1EA9-2C2C-48F2-A929-94FB8D122208}" name="MEL sensitivity" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{551BC3AE-D751-46F6-88A2-090EF8E1ABE8}" name="MEL precision" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{296FC3D5-7186-406D-B2E4-197D9ABFDA03}" name="MEL F1 score" dataDxfId="7"/>
-    <tableColumn id="22" xr3:uid="{E186789E-54B9-4287-83B5-542125F36831}" name="MEL AUC" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{631A4814-AC6D-45DC-9DDA-9C5DCF424C30}" name="SCC Specificity" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{04E21B3C-AB7F-4EFC-BC0C-0F6F185E9EE6}" name="SCC sensitivity" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{D419F5DC-3274-47FE-98C7-089F060E76B3}" name="SCC precision" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C971C848-AE17-4A17-898B-01154D7A5111}" name="SCC F1 score" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{7FFC3286-B391-4AF1-8FCA-4555CB93DA17}" name="SCC AUC " dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{6AF2E814-BA7F-4F43-AAD4-A8D913DDFC87}" name="Best Parameters" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}" name="Table2" displayName="Table2" ref="B13:AC19" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="B13:AC19" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}"/>
+  <tableColumns count="28">
+    <tableColumn id="13" xr3:uid="{6A0F991E-C258-4678-8369-67988AFEA4D6}" name="Experiment Count" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B1948067-CB65-4206-AE71-0D57640D7089}" name="Scoring metric" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{FDDCB198-EAE1-4ED4-A066-F8DBAC98C717}" name="Features" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{83D1AD7E-916A-4241-B599-9349DCDB2027}" name="N_Features" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{70DAF01F-DAE6-4B77-9BDB-7F5053A6F854}" name="Data Shuffled" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{3B5E59E9-2BF5-4D6D-816E-23251AFDB13E}" name="Feature Selection" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{F7473F45-1D6D-409F-9883-1FD36FD545E3}" name="Model" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{90C55BBC-BCBC-4A00-8864-5A767EA01E45}" name="Multiclass handling" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{75867AB3-1849-4FCA-B58F-BE8AEF3B207D}" name="Imbalance handling" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{B2F22562-6078-45C9-A5D5-49F1FBF2A4F1}" name="Accuracy" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{72664E3E-D59C-4D9C-8541-496AB288C8B6}" name="Balanced accuracy" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{0FEE43E7-8EFC-4D86-86B0-C5FE824F8CBB}" name="Weighted f1" dataDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{957B2BF0-94D0-4D47-92EE-5F281E10A28D}" name="BCC Specificity" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{BC24D8AD-88D3-42DE-B472-81BDDB9C87B9}" name="BCC sensitivity" dataDxfId="15"/>
+    <tableColumn id="25" xr3:uid="{69470701-5DB0-4C11-AF39-0426EC578174}" name="BCC precision" dataDxfId="14"/>
+    <tableColumn id="26" xr3:uid="{45ED09DC-26C9-4D46-8786-471740B03DA6}" name="BCC F1 score" dataDxfId="13"/>
+    <tableColumn id="27" xr3:uid="{728ACE6E-7304-449C-A3BC-0DFA6F380155}" name="BCC AUC " dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{99DAD431-5D89-4923-BC81-A35FE3C6B664}" name="MEL Specificity" dataDxfId="11"/>
+    <tableColumn id="19" xr3:uid="{AD2D1EA9-2C2C-48F2-A929-94FB8D122208}" name="MEL sensitivity" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{551BC3AE-D751-46F6-88A2-090EF8E1ABE8}" name="MEL precision" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{296FC3D5-7186-406D-B2E4-197D9ABFDA03}" name="MEL F1 score" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{E186789E-54B9-4287-83B5-542125F36831}" name="MEL AUC" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{631A4814-AC6D-45DC-9DDA-9C5DCF424C30}" name="SCC Specificity" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{04E21B3C-AB7F-4EFC-BC0C-0F6F185E9EE6}" name="SCC sensitivity" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{D419F5DC-3274-47FE-98C7-089F060E76B3}" name="SCC precision" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{C971C848-AE17-4A17-898B-01154D7A5111}" name="SCC F1 score" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{7FFC3286-B391-4AF1-8FCA-4555CB93DA17}" name="SCC AUC " dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{6AF2E814-BA7F-4F43-AAD4-A8D913DDFC87}" name="Best Parameters" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1015,23 +1065,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AC19"/>
+  <dimension ref="B2:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.21875" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.21875" customWidth="1"/>
@@ -1049,10 +1099,11 @@
     <col min="25" max="25" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="32.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1133,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1096,7 +1147,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1110,7 +1161,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1124,7 +1175,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1138,7 +1189,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1152,7 +1203,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1166,7 +1217,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1180,7 +1231,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1194,7 +1245,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1208,7 +1259,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1222,317 +1273,373 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="P13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="Q13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="R13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="S13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="5" t="s">
+      <c r="T13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="U13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="V13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="V13" s="9" t="s">
+      <c r="W13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="W13" s="5" t="s">
+      <c r="X13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="X13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="Z13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="AA13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AA13" s="9" t="s">
+      <c r="AB13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AB13" s="9" t="s">
+      <c r="AC13" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>0</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>0.65275590551181095</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>0.54931695652250601</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>0.65539279537074302</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>0.78886010362694303</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>0.56626506024096301</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>0.63370786516853905</v>
       </c>
-      <c r="P14" s="1">
+      <c r="Q14" s="1">
         <v>0.59809119830328705</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <v>0.67756258193395302</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S14" s="1">
         <v>0.69087837837837796</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <v>0.762536873156342</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>0.73857142857142799</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V14" s="1">
         <v>0.75036284470246695</v>
       </c>
-      <c r="V14" s="1">
+      <c r="W14" s="1">
         <v>0.72670762576736003</v>
       </c>
-      <c r="W14" s="1">
+      <c r="X14" s="1">
         <v>0.91921768707482998</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Y14" s="1">
         <v>0.31914893617021201</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Z14" s="1">
         <v>0.24</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AA14" s="1">
         <v>0.27397260273972601</v>
       </c>
-      <c r="AA14" s="1">
+      <c r="AB14" s="1">
         <v>0.61918331162252105</v>
       </c>
-      <c r="AB14" s="7" t="s">
+      <c r="AC14" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>0</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="I15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>0.74803149606299202</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>0.61236977030068396</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>0.75455430714842497</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>0.82901554404144995</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>0.77911646586345296</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>0.74615384615384595</v>
       </c>
-      <c r="P15" s="1">
+      <c r="Q15" s="1">
         <v>0.76227897838899805</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>0.80406600495245195</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>0.84290540540540504</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <v>0.79203539823008795</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>0.85238095238095202</v>
       </c>
-      <c r="U15" s="1">
+      <c r="V15" s="1">
         <v>0.82110091743119196</v>
       </c>
-      <c r="V15" s="1">
+      <c r="W15" s="1">
         <v>0.817470401817746</v>
       </c>
-      <c r="W15" s="1">
+      <c r="X15" s="1">
         <v>0.91921768707482998</v>
       </c>
-      <c r="X15" s="1">
+      <c r="Y15" s="1">
         <v>0.26595744680851002</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="Z15" s="1">
         <v>0.20833333333333301</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AA15" s="1">
         <v>0.233644859813084</v>
       </c>
-      <c r="AA15" s="1">
+      <c r="AB15" s="1">
         <v>0.59258756694167003</v>
       </c>
-      <c r="AB15" s="1" t="s">
+      <c r="AC15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="6">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
+      <c r="H16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.77244094488188897</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.618591481346209</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.76767329651808902</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.81606217616580301</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0.81526104417670597</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.74087591240875905</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.77629063097514295</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.81566161017125405</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.83108108108108103</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.81710914454277195</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.84709480122324099</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.83183183183183096</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0.82409511281192704</v>
+      </c>
+      <c r="X16" s="1">
+        <v>0.96003401360544205</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>0.22340425531914801</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0.308823529411764</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0.25925925925925902</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0.59171913446229496</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>0</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="1"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="7"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1551,27 +1658,28 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>0</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1590,27 +1698,28 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>0</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="1"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1629,6 +1738,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
train multi-class with latest improvements
</commit_message>
<xml_diff>
--- a/output/train_experiments_results - challenge2.xlsx
+++ b/output/train_experiments_results - challenge2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\master\udg\CAD\project\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdal\Documents\Master\EMJMD MAIA\SEMESTER 3 - UdG\CAD\Melanoma-classification-using-machine-learning\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30485FE6-C1B7-4D2F-835D-57C087ABBB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F920591F-8F51-4D6C-A96B-EC52831CDB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Experiment Count</t>
   </si>
@@ -160,6 +160,51 @@
   </si>
   <si>
     <t>{'C': 1, 'penalty': 'l1', 'solver': 'liblinear'}</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>Color (RGB, HSV, LAB, Gray) 
+from 3 histogram regions + GLCM + LBP</t>
+  </si>
+  <si>
+    <t>SelectBestK</t>
+  </si>
+  <si>
+    <t>100 selected</t>
+  </si>
+  <si>
+    <t>ovr</t>
+  </si>
+  <si>
+    <t>SMOTE oversampling + 
+Random UnderSampling + class_weight='balanced'</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 0.1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>ovo</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>{   'max_depth': 9,
+                           'min_samples_leaf': 1,
+                           'min_samples_split': 2,
+                           'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>XGBOOST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMOTE oversampling + 
+Random UnderSampling </t>
   </si>
 </sst>
 </file>
@@ -288,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,35 +365,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+  <dxfs count="42">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -653,6 +694,19 @@
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
@@ -749,27 +803,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I6" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="B2:I6" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}" name="Table2" displayName="Table2" ref="B13:AC19" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
-  <autoFilter ref="B13:AC19" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}"/>
-  <tableColumns count="28">
-    <tableColumn id="13" xr3:uid="{6A0F991E-C258-4678-8369-67988AFEA4D6}" name="Experiment Count" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}" name="Table2" displayName="Table2" ref="B13:AD23" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
+  <autoFilter ref="B13:AD23" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}"/>
+  <tableColumns count="29">
+    <tableColumn id="13" xr3:uid="{6A0F991E-C258-4678-8369-67988AFEA4D6}" name="Experiment Count" dataDxfId="28"/>
     <tableColumn id="1" xr3:uid="{B1948067-CB65-4206-AE71-0D57640D7089}" name="Scoring metric" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{FDDCB198-EAE1-4ED4-A066-F8DBAC98C717}" name="Features" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{83D1AD7E-916A-4241-B599-9349DCDB2027}" name="N_Features" dataDxfId="25"/>
@@ -779,24 +833,25 @@
     <tableColumn id="7" xr3:uid="{90C55BBC-BCBC-4A00-8864-5A767EA01E45}" name="Multiclass handling" dataDxfId="21"/>
     <tableColumn id="8" xr3:uid="{75867AB3-1849-4FCA-B58F-BE8AEF3B207D}" name="Imbalance handling" dataDxfId="20"/>
     <tableColumn id="9" xr3:uid="{B2F22562-6078-45C9-A5D5-49F1FBF2A4F1}" name="Accuracy" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{72664E3E-D59C-4D9C-8541-496AB288C8B6}" name="Balanced accuracy" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{0FEE43E7-8EFC-4D86-86B0-C5FE824F8CBB}" name="Weighted f1" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{957B2BF0-94D0-4D47-92EE-5F281E10A28D}" name="BCC Specificity" dataDxfId="16"/>
-    <tableColumn id="24" xr3:uid="{BC24D8AD-88D3-42DE-B472-81BDDB9C87B9}" name="BCC sensitivity" dataDxfId="15"/>
-    <tableColumn id="25" xr3:uid="{69470701-5DB0-4C11-AF39-0426EC578174}" name="BCC precision" dataDxfId="14"/>
-    <tableColumn id="26" xr3:uid="{45ED09DC-26C9-4D46-8786-471740B03DA6}" name="BCC F1 score" dataDxfId="13"/>
-    <tableColumn id="27" xr3:uid="{728ACE6E-7304-449C-A3BC-0DFA6F380155}" name="BCC AUC " dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{99DAD431-5D89-4923-BC81-A35FE3C6B664}" name="MEL Specificity" dataDxfId="11"/>
-    <tableColumn id="19" xr3:uid="{AD2D1EA9-2C2C-48F2-A929-94FB8D122208}" name="MEL sensitivity" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{551BC3AE-D751-46F6-88A2-090EF8E1ABE8}" name="MEL precision" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{296FC3D5-7186-406D-B2E4-197D9ABFDA03}" name="MEL F1 score" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{E186789E-54B9-4287-83B5-542125F36831}" name="MEL AUC" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{631A4814-AC6D-45DC-9DDA-9C5DCF424C30}" name="SCC Specificity" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{04E21B3C-AB7F-4EFC-BC0C-0F6F185E9EE6}" name="SCC sensitivity" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{D419F5DC-3274-47FE-98C7-089F060E76B3}" name="SCC precision" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{C971C848-AE17-4A17-898B-01154D7A5111}" name="SCC F1 score" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{7FFC3286-B391-4AF1-8FCA-4555CB93DA17}" name="SCC AUC " dataDxfId="2"/>
-    <tableColumn id="29" xr3:uid="{6AF2E814-BA7F-4F43-AAD4-A8D913DDFC87}" name="Best Parameters" dataDxfId="1"/>
+    <tableColumn id="30" xr3:uid="{A0F03210-DD80-4B4A-B100-07FBD77B98FC}" name="Kappa" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{72664E3E-D59C-4D9C-8541-496AB288C8B6}" name="Balanced accuracy" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{0FEE43E7-8EFC-4D86-86B0-C5FE824F8CBB}" name="Weighted f1" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{957B2BF0-94D0-4D47-92EE-5F281E10A28D}" name="BCC Specificity" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{BC24D8AD-88D3-42DE-B472-81BDDB9C87B9}" name="BCC sensitivity" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{69470701-5DB0-4C11-AF39-0426EC578174}" name="BCC precision" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{45ED09DC-26C9-4D46-8786-471740B03DA6}" name="BCC F1 score" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{728ACE6E-7304-449C-A3BC-0DFA6F380155}" name="BCC AUC " dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{99DAD431-5D89-4923-BC81-A35FE3C6B664}" name="MEL Specificity" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{AD2D1EA9-2C2C-48F2-A929-94FB8D122208}" name="MEL sensitivity" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{551BC3AE-D751-46F6-88A2-090EF8E1ABE8}" name="MEL precision" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{296FC3D5-7186-406D-B2E4-197D9ABFDA03}" name="MEL F1 score" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{E186789E-54B9-4287-83B5-542125F36831}" name="MEL AUC" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{631A4814-AC6D-45DC-9DDA-9C5DCF424C30}" name="SCC Specificity" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{04E21B3C-AB7F-4EFC-BC0C-0F6F185E9EE6}" name="SCC sensitivity" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{D419F5DC-3274-47FE-98C7-089F060E76B3}" name="SCC precision" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C971C848-AE17-4A17-898B-01154D7A5111}" name="SCC F1 score" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{7FFC3286-B391-4AF1-8FCA-4555CB93DA17}" name="SCC AUC " dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{6AF2E814-BA7F-4F43-AAD4-A8D913DDFC87}" name="Best Parameters" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1065,45 +1120,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AD19"/>
+  <dimension ref="B2:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC26"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" customWidth="1"/>
-    <col min="10" max="10" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.21875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="17.5546875" customWidth="1"/>
-    <col min="16" max="16" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.21875" customWidth="1"/>
-    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1796875" customWidth="1"/>
+    <col min="10" max="10" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.08984375" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1796875" customWidth="1"/>
+    <col min="15" max="15" width="14.36328125" customWidth="1"/>
+    <col min="16" max="16" width="17.54296875" customWidth="1"/>
+    <col min="17" max="17" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1796875" customWidth="1"/>
+    <col min="23" max="23" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" customWidth="1"/>
+    <col min="25" max="25" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1132,8 +1188,9 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1146,8 +1203,9 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1160,8 +1218,9 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1174,8 +1233,9 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1188,8 +1248,9 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1202,8 +1263,9 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1216,8 +1278,9 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1230,8 +1293,9 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1244,8 +1308,9 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1258,8 +1323,9 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1272,8 +1338,9 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
@@ -1305,65 +1372,68 @@
         <v>6</v>
       </c>
       <c r="L13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="P13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="Q13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="R13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="S13" s="5" t="s">
+      <c r="T13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="U13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="V13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="V13" s="5" t="s">
+      <c r="W13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W13" s="9" t="s">
+      <c r="X13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="X13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="Z13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="AA13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="AB13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AB13" s="9" t="s">
+      <c r="AC13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AC13" s="9" t="s">
+      <c r="AD13" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <v>0</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1390,66 +1460,67 @@
       <c r="K14" s="1">
         <v>0.65275590551181095</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1">
         <v>0.54931695652250601</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>0.65539279537074302</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>0.78886010362694303</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>0.56626506024096301</v>
       </c>
-      <c r="P14" s="1">
+      <c r="Q14" s="1">
         <v>0.63370786516853905</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <v>0.59809119830328705</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S14" s="1">
         <v>0.67756258193395302</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <v>0.69087837837837796</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>0.762536873156342</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V14" s="1">
         <v>0.73857142857142799</v>
       </c>
-      <c r="V14" s="1">
+      <c r="W14" s="1">
         <v>0.75036284470246695</v>
       </c>
-      <c r="W14" s="1">
+      <c r="X14" s="1">
         <v>0.72670762576736003</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Y14" s="1">
         <v>0.91921768707482998</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Z14" s="1">
         <v>0.31914893617021201</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AA14" s="1">
         <v>0.24</v>
       </c>
-      <c r="AA14" s="1">
+      <c r="AB14" s="1">
         <v>0.27397260273972601</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AC14" s="1">
         <v>0.61918331162252105</v>
       </c>
-      <c r="AC14" s="7" t="s">
+      <c r="AD14" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>0</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1476,69 +1547,70 @@
       <c r="K15" s="1">
         <v>0.74803149606299202</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1">
         <v>0.61236977030068396</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>0.75455430714842497</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>0.82901554404144995</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>0.77911646586345296</v>
       </c>
-      <c r="P15" s="1">
+      <c r="Q15" s="1">
         <v>0.74615384615384595</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>0.76227897838899805</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>0.80406600495245195</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <v>0.84290540540540504</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>0.79203539823008795</v>
       </c>
-      <c r="U15" s="1">
+      <c r="V15" s="1">
         <v>0.85238095238095202</v>
       </c>
-      <c r="V15" s="1">
+      <c r="W15" s="1">
         <v>0.82110091743119196</v>
       </c>
-      <c r="W15" s="1">
+      <c r="X15" s="1">
         <v>0.817470401817746</v>
       </c>
-      <c r="X15" s="1">
+      <c r="Y15" s="1">
         <v>0.91921768707482998</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="Z15" s="1">
         <v>0.26595744680851002</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AA15" s="1">
         <v>0.20833333333333301</v>
       </c>
-      <c r="AA15" s="1">
+      <c r="AB15" s="1">
         <v>0.233644859813084</v>
       </c>
-      <c r="AB15" s="1">
+      <c r="AC15" s="1">
         <v>0.59258756694167003</v>
       </c>
-      <c r="AC15" s="1" t="s">
+      <c r="AD15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>0</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1565,66 +1637,67 @@
       <c r="K16" s="1">
         <v>0.77244094488188897</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1">
         <v>0.618591481346209</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>0.76767329651808902</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>0.81606217616580301</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>0.81526104417670597</v>
       </c>
-      <c r="P16" s="1">
+      <c r="Q16" s="1">
         <v>0.74087591240875905</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>0.77629063097514295</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <v>0.81566161017125405</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T16" s="1">
         <v>0.83108108108108103</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U16" s="1">
         <v>0.81710914454277195</v>
       </c>
-      <c r="U16" s="1">
+      <c r="V16" s="1">
         <v>0.84709480122324099</v>
       </c>
-      <c r="V16" s="1">
+      <c r="W16" s="1">
         <v>0.83183183183183096</v>
       </c>
-      <c r="W16" s="1">
+      <c r="X16" s="1">
         <v>0.82409511281192704</v>
       </c>
-      <c r="X16" s="1">
+      <c r="Y16" s="1">
         <v>0.96003401360544205</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="Z16" s="1">
         <v>0.22340425531914801</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="AA16" s="1">
         <v>0.308823529411764</v>
       </c>
-      <c r="AA16" s="1">
+      <c r="AB16" s="1">
         <v>0.25925925925925902</v>
       </c>
-      <c r="AB16" s="1">
+      <c r="AC16" s="1">
         <v>0.59171913446229496</v>
       </c>
-      <c r="AC16" s="1" t="s">
+      <c r="AD16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>0</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1659,12 +1732,13 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B18" s="6">
         <v>0</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1699,12 +1773,13 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>0</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1739,6 +1814,323 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+    </row>
+    <row r="20" spans="2:30" ht="58" x14ac:dyDescent="0.35">
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0.81338582677165305</v>
+      </c>
+      <c r="L20" s="13">
+        <v>0.65350079432689401</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0.67310212418115301</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0.80545728728870403</v>
+      </c>
+      <c r="O20" s="13">
+        <v>0.86269430051813401</v>
+      </c>
+      <c r="P20" s="13">
+        <v>0.79718875502008002</v>
+      </c>
+      <c r="Q20" s="13">
+        <v>0.78926441351888599</v>
+      </c>
+      <c r="R20" s="13">
+        <v>0.79320679320679299</v>
+      </c>
+      <c r="S20" s="13">
+        <v>0.82994152776910701</v>
+      </c>
+      <c r="T20" s="13">
+        <v>0.80236486486486402</v>
+      </c>
+      <c r="U20" s="13">
+        <v>0.89233038348082505</v>
+      </c>
+      <c r="V20" s="13">
+        <v>0.83795013850415501</v>
+      </c>
+      <c r="W20" s="13">
+        <v>0.86428571428571399</v>
+      </c>
+      <c r="X20" s="13">
+        <v>0.84734762417284504</v>
+      </c>
+      <c r="Y20" s="13">
+        <v>0.98809523809523803</v>
+      </c>
+      <c r="Z20" s="13">
+        <v>0.329787234042553</v>
+      </c>
+      <c r="AA20" s="13">
+        <v>0.688888888888888</v>
+      </c>
+      <c r="AB20" s="13">
+        <v>0.44604316546762501</v>
+      </c>
+      <c r="AC20" s="13">
+        <v>0.65894123606889499</v>
+      </c>
+      <c r="AD20" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" ht="58" x14ac:dyDescent="0.35">
+      <c r="B21" s="6">
+        <v>2</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0.81338582677165305</v>
+      </c>
+      <c r="L21" s="13">
+        <v>0.65350079432689401</v>
+      </c>
+      <c r="M21" s="13">
+        <v>0.67310212418115301</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0.80545728728870403</v>
+      </c>
+      <c r="O21" s="13">
+        <v>0.86269430051813401</v>
+      </c>
+      <c r="P21" s="13">
+        <v>0.79718875502008002</v>
+      </c>
+      <c r="Q21" s="13">
+        <v>0.78926441351888599</v>
+      </c>
+      <c r="R21" s="13">
+        <v>0.79320679320679299</v>
+      </c>
+      <c r="S21" s="13">
+        <v>0.82994152776910701</v>
+      </c>
+      <c r="T21" s="13">
+        <v>0.80236486486486402</v>
+      </c>
+      <c r="U21" s="13">
+        <v>0.89233038348082505</v>
+      </c>
+      <c r="V21" s="13">
+        <v>0.83795013850415501</v>
+      </c>
+      <c r="W21" s="13">
+        <v>0.86428571428571399</v>
+      </c>
+      <c r="X21" s="13">
+        <v>0.84734762417284504</v>
+      </c>
+      <c r="Y21" s="13">
+        <v>0.98809523809523803</v>
+      </c>
+      <c r="Z21" s="13">
+        <v>0.329787234042553</v>
+      </c>
+      <c r="AA21" s="13">
+        <v>0.688888888888888</v>
+      </c>
+      <c r="AB21" s="13">
+        <v>0.44604316546762501</v>
+      </c>
+      <c r="AC21" s="13">
+        <v>0.65894123606889499</v>
+      </c>
+      <c r="AD21" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" ht="58" x14ac:dyDescent="0.35">
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="12"/>
+      <c r="J22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0.74881889763779497</v>
+      </c>
+      <c r="L22" s="13">
+        <v>0.556769944422563</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0.64397261423778296</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0.75400758373277899</v>
+      </c>
+      <c r="O22" s="13">
+        <v>0.80051813471502498</v>
+      </c>
+      <c r="P22" s="13">
+        <v>0.75100401606425704</v>
+      </c>
+      <c r="Q22" s="13">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="R22" s="13">
+        <v>0.72904483430799205</v>
+      </c>
+      <c r="S22" s="13">
+        <v>0.77576107538964101</v>
+      </c>
+      <c r="T22" s="13">
+        <v>0.85472972972972905</v>
+      </c>
+      <c r="U22" s="13">
+        <v>0.79793510324483696</v>
+      </c>
+      <c r="V22" s="13">
+        <v>0.86283891547049396</v>
+      </c>
+      <c r="W22" s="13">
+        <v>0.82911877394636002</v>
+      </c>
+      <c r="X22" s="13">
+        <v>0.82633241648728295</v>
+      </c>
+      <c r="Y22" s="13">
+        <v>0.93282312925169997</v>
+      </c>
+      <c r="Z22" s="13">
+        <v>0.38297872340425498</v>
+      </c>
+      <c r="AA22" s="13">
+        <v>0.31304347826086898</v>
+      </c>
+      <c r="AB22" s="13">
+        <v>0.34449760765550203</v>
+      </c>
+      <c r="AC22" s="13">
+        <v>0.65790092632797703</v>
+      </c>
+      <c r="AD22" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="12"/>
+      <c r="J23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="13">
+        <v>0.80078740157480299</v>
+      </c>
+      <c r="L23" s="13">
+        <v>0.63205520488837097</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="13"/>
+      <c r="AD23" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>